<commit_message>
- Actualizada branch de entrega con CP/Monticulo y PilaEstatica con resize.
</commit_message>
<xml_diff>
--- a/practica2/branches/entregaTP2/TDAs/doc/metricas/metricas_cola.xlsx
+++ b/practica2/branches/entregaTP2/TDAs/doc/metricas/metricas_cola.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="1785" windowWidth="16380" windowHeight="8190" tabRatio="329"/>
+    <workbookView xWindow="15" yWindow="30" windowWidth="28680" windowHeight="12330" tabRatio="329"/>
   </bookViews>
   <sheets>
     <sheet name="Metricas" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -107,6 +107,15 @@
   </si>
   <si>
     <t>Implementar ColaHL</t>
+  </si>
+  <si>
+    <t>Implementar Monticulo</t>
+  </si>
+  <si>
+    <t>Implementar MonticuloMaximo</t>
+  </si>
+  <si>
+    <t>Implementar ColaPrioridad</t>
   </si>
 </sst>
 </file>
@@ -672,7 +681,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -709,9 +718,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="21" fontId="5" fillId="5" borderId="17" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="4" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1088,7 +1094,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Metricas!$A$22:$A$23</c:f>
+              <c:f>Metricas!$A$25:$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1102,15 +1108,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Metricas!$C$22:$C$23</c:f>
+              <c:f>Metricas!$C$25:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.6153846153846118E-2</c:v>
+                  <c:v>7.6923076923076913E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.90384615384615385</c:v>
+                  <c:v>0.92307692307692302</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1152,13 +1158,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1695,10 +1701,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:IU40"/>
+  <dimension ref="A1:IU43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1716,30 +1722,30 @@
     <col min="11" max="255" width="34.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="52" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="54">
+      <c r="B2" s="53">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="C2" s="11">
@@ -1753,7 +1759,7 @@
         <v>0.4826388888888889</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1771,41 +1777,41 @@
         <v>0.53611111111111109</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46" t="s">
+    <row r="4" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="48" t="s">
+      <c r="J5" s="47" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="16">
@@ -1833,12 +1839,12 @@
       <c r="I6" s="17">
         <v>0</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="30">
         <f>G6+I6</f>
         <v>3.4722222222222099E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>27</v>
       </c>
@@ -1857,8 +1863,8 @@
       <c r="F7" s="8">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G7" s="8">
-        <f>F7-E7</f>
+      <c r="G7" s="17">
+        <f t="shared" ref="G7:G16" si="0">F7-E7</f>
         <v>2.9861111111111172E-2</v>
       </c>
       <c r="H7" s="7">
@@ -1867,12 +1873,12 @@
       <c r="I7" s="8">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="J7" s="19">
-        <f>G7+I7</f>
+      <c r="J7" s="30">
+        <f t="shared" ref="J7:J16" si="1">G7+I7</f>
         <v>4.0277777777777836E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>28</v>
       </c>
@@ -1891,8 +1897,8 @@
       <c r="F8" s="8">
         <v>0.1451388888888889</v>
       </c>
-      <c r="G8" s="8">
-        <f>F8-E8</f>
+      <c r="G8" s="17">
+        <f t="shared" si="0"/>
         <v>2.569444444444445E-2</v>
       </c>
       <c r="H8" s="7">
@@ -1901,12 +1907,12 @@
       <c r="I8" s="8">
         <v>0</v>
       </c>
-      <c r="J8" s="19">
-        <f>G8+I8</f>
+      <c r="J8" s="30">
+        <f t="shared" si="1"/>
         <v>2.569444444444445E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>29</v>
       </c>
@@ -1925,8 +1931,8 @@
       <c r="F9" s="8">
         <v>0.67499999999999993</v>
       </c>
-      <c r="G9" s="8">
-        <f t="shared" ref="G9:G13" si="0">F9-E9</f>
+      <c r="G9" s="17">
+        <f t="shared" si="0"/>
         <v>1.2499999999999956E-2</v>
       </c>
       <c r="H9" s="7">
@@ -1935,12 +1941,12 @@
       <c r="I9" s="8">
         <v>0</v>
       </c>
-      <c r="J9" s="19">
-        <f t="shared" ref="J9:J13" si="1">G9+I9</f>
+      <c r="J9" s="30">
+        <f t="shared" si="1"/>
         <v>1.2499999999999956E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>30</v>
       </c>
@@ -1959,7 +1965,7 @@
       <c r="F10" s="8">
         <v>0.52847222222222223</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="17">
         <f t="shared" si="0"/>
         <v>2.6388888888888906E-2</v>
       </c>
@@ -1969,198 +1975,300 @@
       <c r="I10" s="8">
         <v>0</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="30">
         <f t="shared" si="1"/>
         <v>2.6388888888888906E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="7">
+        <v>20</v>
+      </c>
+      <c r="C11" s="7">
+        <v>6</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.81180555555555556</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.81597222222222221</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666519E-3</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0</v>
+      </c>
+      <c r="J11" s="30">
+        <f t="shared" si="1"/>
+        <v>4.1666666666666519E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="7">
+        <v>50</v>
+      </c>
+      <c r="C12" s="7">
+        <v>103</v>
+      </c>
+      <c r="D12" s="8">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.81597222222222221</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.87569444444444444</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" si="0"/>
+        <v>5.9722222222222232E-2</v>
+      </c>
+      <c r="H12" s="7">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="J12" s="30">
+        <f t="shared" si="1"/>
+        <v>6.3194444444444456E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="7">
+        <v>40</v>
+      </c>
+      <c r="C13" s="7">
+        <v>47</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.73402777777777783</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.73888888888888893</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="0"/>
+        <v>4.8611111111110938E-3</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0</v>
+      </c>
+      <c r="J13" s="30">
+        <f t="shared" si="1"/>
+        <v>4.8611111111110938E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="19">
+      <c r="H14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="19">
+      <c r="H15" s="7"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="8">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="19">
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49" t="s">
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="25">
-        <f>SUM(B6:B13)</f>
-        <v>257</v>
-      </c>
-      <c r="C14" s="25">
-        <f>SUM(C6:C13)</f>
-        <v>287</v>
-      </c>
-      <c r="D14" s="26">
-        <f>SUM(D6:D13)</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26">
-        <f>SUM(G6:G13)</f>
-        <v>9.7916666666666693E-2</v>
-      </c>
-      <c r="H14" s="27">
-        <f>SUM(H6:H13)</f>
-        <v>1</v>
-      </c>
-      <c r="I14" s="28">
-        <f>SUM(I6:I13)</f>
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="J14" s="29">
-        <f>SUM(J6:J13)</f>
-        <v>0.10833333333333336</v>
-      </c>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="50" t="s">
+      <c r="B17" s="24">
+        <f>SUM(B6:B16)</f>
+        <v>367</v>
+      </c>
+      <c r="C17" s="24">
+        <f>SUM(C6:C16)</f>
+        <v>443</v>
+      </c>
+      <c r="D17" s="25">
+        <f>SUM(D6:D16)</f>
+        <v>0.13888888888888887</v>
+      </c>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="25">
+        <f>SUM(G6:G16)</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="H17" s="26">
+        <f>SUM(H6:H16)</f>
+        <v>2</v>
+      </c>
+      <c r="I17" s="27">
+        <f>SUM(I6:I16)</f>
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="J17" s="28">
+        <f>SUM(J6:J16)</f>
+        <v>0.18055555555555558</v>
+      </c>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="21">
-        <f>IF(EXACT($C$14, 0),"-",ABS($B$14-$C$14)/$C$14)</f>
-        <v>0.10452961672473868</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="43" t="s">
+      <c r="B18" s="20">
+        <f>IF(EXACT($C$17, 0),"-",ABS($B$17-$C$17)/$C$17)</f>
+        <v>0.17155756207674944</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="44"/>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="B20" s="43"/>
+    </row>
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="33">
-        <f>C14</f>
-        <v>287</v>
-      </c>
-      <c r="C18" s="9"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="B21" s="32">
+        <f>C17</f>
+        <v>443</v>
+      </c>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="35">
-        <f>IF(EXACT($B$18,0),"-",$B$18/((J14-INT(J14))*24))</f>
-        <v>110.38461538461536</v>
-      </c>
-      <c r="C19" s="9"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="36" t="s">
+      <c r="B22" s="34">
+        <f>IF(EXACT($B$21,0),"-",$B$21/((J17-INT(J17))*24))</f>
+        <v>102.23076923076921</v>
+      </c>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="35">
-        <f>IF(EXACT($B$18,0),"-",H14/($B$18/10))</f>
-        <v>3.484320557491289E-2</v>
-      </c>
-      <c r="C20" s="9"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="36" t="s">
+      <c r="B23" s="34">
+        <f>IF(EXACT($B$21,0),"-",H17/($B$21/10))</f>
+        <v>4.5146726862302484E-2</v>
+      </c>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="37">
-        <f>IF(EXACT($B$18,0),"-",H14/$B$18)</f>
-        <v>3.4843205574912892E-3</v>
-      </c>
-      <c r="C21" s="45" t="s">
+      <c r="B24" s="36">
+        <f>IF(EXACT($B$21,0),"-",H17/$B$21)</f>
+        <v>4.5146726862302479E-3</v>
+      </c>
+      <c r="C24" s="44" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="38">
-        <f>I14</f>
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="C22" s="41">
-        <f>IF(EXACT(J14,0),5%,B22/J14)</f>
-        <v>9.6153846153846118E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="39" t="s">
+      <c r="B25" s="37">
+        <f>I17</f>
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C25" s="40">
+        <f>IF(EXACT(J17,0),5%,B25/J17)</f>
+        <v>7.6923076923076913E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="40">
-        <f>G14</f>
-        <v>9.7916666666666693E-2</v>
-      </c>
-      <c r="C23" s="42">
-        <f>IF(EXACT(J14,0),95%,B23/J14)</f>
-        <v>0.90384615384615385</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="6"/>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C38" s="4"/>
-    </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D40" s="4"/>
+      <c r="B26" s="39">
+        <f>G17</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="C26" s="41">
+        <f>IF(EXACT(J17,0),95%,B26/J17)</f>
+        <v>0.92307692307692302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D28" s="6"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C41" s="4"/>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="4"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>